<commit_message>
2021-09-16 Added story point to User stories
</commit_message>
<xml_diff>
--- a/Documentation/TestCaseTable.xlsx
+++ b/Documentation/TestCaseTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNI\Second Year\ITS\INDIVIDUAL PROJECT\simplehomes-s3\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7CBFF89-1F65-4CC5-A8A5-27CDE51573DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A62F0CC-BA69-4B16-A715-7FB6FAC6088E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12528" xr2:uid="{6B7E2DC7-9843-404D-A7AE-4406DCB0DAA1}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{6B7E2DC7-9843-404D-A7AE-4406DCB0DAA1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -817,7 +817,7 @@
   <dimension ref="B2:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="B2:G6"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>